<commit_message>
Relaxed R4 (average 48 hours acceptable)
</commit_message>
<xml_diff>
--- a/apps/duty-roster-solver-files/duty_roster_input_template_0630_no_div.xlsx
+++ b/apps/duty-roster-solver-files/duty_roster_input_template_0630_no_div.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rng/Documents/VSCode_Workspace/marimo_ngs/apps/duty-roster-solver-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36902507-0977-AB4C-BDA7-9941BCC22E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE065AE1-D599-7647-87BF-3A4C41DBFAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="28800" windowHeight="18000" xr2:uid="{CC6AE4C9-93E2-014C-AFB4-2BE1C15F0665}"/>
   </bookViews>
@@ -642,8 +642,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C220"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -699,21 +699,21 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3">
-        <v>45965</v>
+        <v>45964</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3">
-        <v>45965</v>
+        <v>45964</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -721,10 +721,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3">
-        <v>45965</v>
+        <v>45964</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -732,21 +732,21 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3">
-        <v>45966</v>
+        <v>45964</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3">
-        <v>45966</v>
+        <v>45964</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -754,10 +754,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3">
-        <v>45966</v>
+        <v>45964</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -765,32 +765,32 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3">
-        <v>45967</v>
+        <v>45964</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3">
-        <v>45967</v>
+        <v>45965</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3">
-        <v>45967</v>
+        <v>45965</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -798,32 +798,32 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3">
-        <v>45968</v>
+        <v>45965</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3">
-        <v>45968</v>
+        <v>45965</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3">
-        <v>45968</v>
+        <v>45965</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
@@ -831,21 +831,21 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3">
-        <v>45969</v>
+        <v>45965</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3">
-        <v>45969</v>
+        <v>45965</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
@@ -853,10 +853,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3">
-        <v>45969</v>
+        <v>45965</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -864,10 +864,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3">
-        <v>45970</v>
+        <v>45965</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -875,10 +875,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3">
-        <v>45970</v>
+        <v>45965</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3">
-        <v>45971</v>
+        <v>45966</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>4</v>
@@ -897,7 +897,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3">
-        <v>45971</v>
+        <v>45966</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>27</v>
@@ -908,7 +908,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3">
-        <v>45971</v>
+        <v>45966</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>28</v>
@@ -919,21 +919,21 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3">
-        <v>45972</v>
+        <v>45966</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C25" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3">
-        <v>45972</v>
+        <v>45966</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
@@ -941,21 +941,21 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="3">
-        <v>45973</v>
+        <v>45966</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3">
-        <v>45973</v>
+        <v>45966</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2">
         <v>1</v>
@@ -963,10 +963,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="3">
-        <v>45973</v>
+        <v>45966</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -974,21 +974,21 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="3">
-        <v>45974</v>
+        <v>45966</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C30" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3">
-        <v>45974</v>
+        <v>45966</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C31" s="2">
         <v>1</v>
@@ -996,32 +996,32 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="3">
-        <v>45974</v>
+        <v>45967</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C32" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="3">
-        <v>45975</v>
+        <v>45967</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="C33" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="3">
-        <v>45975</v>
+        <v>45967</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
@@ -1029,10 +1029,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="3">
-        <v>45975</v>
+        <v>45967</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
@@ -1040,21 +1040,21 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="3">
-        <v>45976</v>
+        <v>45967</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C36" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="3">
-        <v>45976</v>
+        <v>45967</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C37" s="2">
         <v>1</v>
@@ -1062,10 +1062,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="3">
-        <v>45976</v>
+        <v>45967</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C38" s="2">
         <v>1</v>
@@ -1073,21 +1073,21 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="3">
-        <v>45977</v>
+        <v>45967</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C39" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3">
-        <v>45977</v>
+        <v>45967</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C40" s="2">
         <v>1</v>
@@ -1095,32 +1095,32 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3">
-        <v>45977</v>
+        <v>45968</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C41" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="3">
-        <v>45964</v>
+        <v>45968</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C42" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="3">
-        <v>45964</v>
+        <v>45968</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -1128,32 +1128,32 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="3">
-        <v>45964</v>
+        <v>45968</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C44" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="3">
-        <v>45965</v>
+        <v>45968</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C45" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="3">
-        <v>45965</v>
+        <v>45968</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C46" s="2">
         <v>1</v>
@@ -1161,10 +1161,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="3">
-        <v>45965</v>
+        <v>45968</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C47" s="2">
         <v>1</v>
@@ -1172,21 +1172,21 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="3">
-        <v>45966</v>
+        <v>45968</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C48" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="3">
-        <v>45966</v>
+        <v>45968</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C49" s="2">
         <v>1</v>
@@ -1194,10 +1194,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="3">
-        <v>45966</v>
+        <v>45968</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C50" s="2">
         <v>1</v>
@@ -1205,10 +1205,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="3">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C51" s="2">
         <v>1</v>
@@ -1216,10 +1216,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="3">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C52" s="2">
         <v>1</v>
@@ -1230,29 +1230,29 @@
         <v>45968</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C53" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="3">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C54" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="3">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C55" s="2">
         <v>1</v>
@@ -1263,10 +1263,10 @@
         <v>45969</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C56" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1274,10 +1274,10 @@
         <v>45969</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C57" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1285,7 +1285,7 @@
         <v>45969</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="2">
         <v>1</v>
@@ -1296,7 +1296,7 @@
         <v>45969</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C59" s="2">
         <v>1</v>
@@ -1307,7 +1307,7 @@
         <v>45969</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C60" s="2">
         <v>1</v>
@@ -1315,10 +1315,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="3">
-        <v>45970</v>
+        <v>45969</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C61" s="2">
         <v>1</v>
@@ -1326,32 +1326,32 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="3">
-        <v>45970</v>
+        <v>45969</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C62" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="3">
-        <v>45970</v>
+        <v>45969</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C63" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="3">
-        <v>45970</v>
+        <v>45969</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C64" s="2">
         <v>1</v>
@@ -1359,10 +1359,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="3">
-        <v>45970</v>
+        <v>45969</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C65" s="2">
         <v>1</v>
@@ -1370,10 +1370,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="3">
-        <v>45970</v>
+        <v>45969</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C66" s="2">
         <v>1</v>
@@ -1381,21 +1381,21 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="3">
-        <v>45971</v>
+        <v>45969</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C67" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="3">
-        <v>45971</v>
+        <v>45969</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C68" s="2">
         <v>1</v>
@@ -1403,21 +1403,21 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="3">
-        <v>45971</v>
+        <v>45969</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C69" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="3">
-        <v>45971</v>
+        <v>45970</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C70" s="2">
         <v>1</v>
@@ -1425,10 +1425,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="3">
-        <v>45971</v>
+        <v>45970</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C71" s="2">
         <v>1</v>
@@ -1436,10 +1436,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="3">
-        <v>45971</v>
+        <v>45970</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C72" s="2">
         <v>1</v>
@@ -1447,21 +1447,21 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="3">
-        <v>45971</v>
+        <v>45970</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C73" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="3">
-        <v>45972</v>
+        <v>45970</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C74" s="2">
         <v>1</v>
@@ -1469,21 +1469,21 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="3">
-        <v>45972</v>
+        <v>45970</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C75" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="3">
-        <v>45972</v>
+        <v>45970</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C76" s="2">
         <v>1</v>
@@ -1491,10 +1491,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="3">
-        <v>45972</v>
+        <v>45970</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C77" s="2">
         <v>1</v>
@@ -1502,10 +1502,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="3">
-        <v>45972</v>
+        <v>45970</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C78" s="2">
         <v>1</v>
@@ -1513,10 +1513,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="3">
-        <v>45972</v>
+        <v>45970</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C79" s="2">
         <v>1</v>
@@ -1524,10 +1524,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="3">
-        <v>45973</v>
+        <v>45970</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C80" s="2">
         <v>1</v>
@@ -1535,21 +1535,21 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="3">
-        <v>45973</v>
+        <v>45970</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C81" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="3">
-        <v>45973</v>
+        <v>45970</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C82" s="2">
         <v>1</v>
@@ -1557,10 +1557,10 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="3">
-        <v>45973</v>
+        <v>45970</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C83" s="2">
         <v>1</v>
@@ -1568,10 +1568,10 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="3">
-        <v>45973</v>
+        <v>45970</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C84" s="2">
         <v>1</v>
@@ -1579,54 +1579,54 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="3">
-        <v>45973</v>
+        <v>45971</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C85" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="3">
-        <v>45974</v>
+        <v>45971</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C86" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="3">
-        <v>45974</v>
+        <v>45971</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C87" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="3">
-        <v>45974</v>
+        <v>45971</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="C88" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="3">
-        <v>45974</v>
+        <v>45971</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C89" s="2">
         <v>1</v>
@@ -1634,21 +1634,21 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="3">
-        <v>45974</v>
+        <v>45971</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C90" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="3">
-        <v>45974</v>
+        <v>45971</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C91" s="2">
         <v>1</v>
@@ -1656,10 +1656,10 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="3">
-        <v>45974</v>
+        <v>45971</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C92" s="2">
         <v>1</v>
@@ -1667,43 +1667,43 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="3">
-        <v>45975</v>
+        <v>45971</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C93" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="3">
-        <v>45975</v>
+        <v>45971</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C94" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="3">
-        <v>45975</v>
+        <v>45971</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C95" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="3">
-        <v>45975</v>
+        <v>45971</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C96" s="2">
         <v>1</v>
@@ -1711,10 +1711,10 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="3">
-        <v>45975</v>
+        <v>45971</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C97" s="2">
         <v>1</v>
@@ -1722,10 +1722,10 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="3">
-        <v>45975</v>
+        <v>45971</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C98" s="2">
         <v>1</v>
@@ -1733,10 +1733,10 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="3">
-        <v>45975</v>
+        <v>45971</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C99" s="2">
         <v>1</v>
@@ -1744,32 +1744,32 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="3">
-        <v>45976</v>
+        <v>45971</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C100" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="3">
-        <v>45976</v>
+        <v>45971</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C101" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="3">
-        <v>45976</v>
+        <v>45971</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C102" s="2">
         <v>1</v>
@@ -1777,10 +1777,10 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="3">
-        <v>45976</v>
+        <v>45971</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C103" s="2">
         <v>1</v>
@@ -1788,10 +1788,10 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="3">
-        <v>45976</v>
+        <v>45971</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C104" s="2">
         <v>1</v>
@@ -1799,10 +1799,10 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="3">
-        <v>45976</v>
+        <v>45972</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C105" s="2">
         <v>1</v>
@@ -1810,43 +1810,43 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="3">
-        <v>45977</v>
+        <v>45972</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C106" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="3">
-        <v>45977</v>
+        <v>45972</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C107" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="3">
-        <v>45977</v>
+        <v>45972</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C108" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="3">
-        <v>45977</v>
+        <v>45972</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C109" s="2">
         <v>1</v>
@@ -1854,10 +1854,10 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="3">
-        <v>45977</v>
+        <v>45972</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C110" s="2">
         <v>1</v>
@@ -1865,10 +1865,10 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="3">
-        <v>45977</v>
+        <v>45972</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C111" s="2">
         <v>1</v>
@@ -1876,10 +1876,10 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="3">
-        <v>45964</v>
+        <v>45972</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C112" s="2">
         <v>1</v>
@@ -1887,21 +1887,21 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="3">
-        <v>45964</v>
+        <v>45972</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C113" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="3">
-        <v>45965</v>
+        <v>45972</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C114" s="2">
         <v>1</v>
@@ -1909,10 +1909,10 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="3">
-        <v>45965</v>
+        <v>45972</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C115" s="2">
         <v>1</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="3">
-        <v>45966</v>
+        <v>45972</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>33</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="3">
-        <v>45966</v>
+        <v>45972</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>34</v>
@@ -1942,10 +1942,10 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="3">
-        <v>45967</v>
+        <v>45972</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C118" s="2">
         <v>1</v>
@@ -1953,10 +1953,10 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="3">
-        <v>45967</v>
+        <v>45972</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C119" s="2">
         <v>1</v>
@@ -1964,10 +1964,10 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="3">
-        <v>45968</v>
+        <v>45972</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C120" s="2">
         <v>1</v>
@@ -1975,10 +1975,10 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="3">
-        <v>45968</v>
+        <v>45972</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C121" s="2">
         <v>1</v>
@@ -1986,10 +1986,10 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="3">
-        <v>45968</v>
+        <v>45972</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C122" s="2">
         <v>1</v>
@@ -1997,21 +1997,21 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="3">
-        <v>45968</v>
+        <v>45973</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C123" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="3">
-        <v>45968</v>
+        <v>45973</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C124" s="2">
         <v>1</v>
@@ -2019,10 +2019,10 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="3">
-        <v>45969</v>
+        <v>45973</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C125" s="2">
         <v>1</v>
@@ -2030,32 +2030,32 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="3">
-        <v>45969</v>
+        <v>45973</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C126" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="3">
-        <v>45969</v>
+        <v>45973</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="C127" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="3">
-        <v>45969</v>
+        <v>45973</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C128" s="2">
         <v>1</v>
@@ -2063,10 +2063,10 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="3">
-        <v>45969</v>
+        <v>45973</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C129" s="2">
         <v>1</v>
@@ -2074,10 +2074,10 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="3">
-        <v>45969</v>
+        <v>45973</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C130" s="2">
         <v>1</v>
@@ -2085,10 +2085,10 @@
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="3">
-        <v>45970</v>
+        <v>45973</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C131" s="2">
         <v>1</v>
@@ -2096,21 +2096,21 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="3">
-        <v>45970</v>
+        <v>45973</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C132" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="3">
-        <v>45970</v>
+        <v>45973</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C133" s="2">
         <v>1</v>
@@ -2118,10 +2118,10 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="3">
-        <v>45970</v>
+        <v>45973</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C134" s="2">
         <v>1</v>
@@ -2129,10 +2129,10 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="3">
-        <v>45970</v>
+        <v>45973</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C135" s="2">
         <v>1</v>
@@ -2140,21 +2140,21 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="3">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C136" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="3">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C137" s="2">
         <v>1</v>
@@ -2162,10 +2162,10 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="3">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C138" s="2">
         <v>1</v>
@@ -2173,10 +2173,10 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="3">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C139" s="2">
         <v>1</v>
@@ -2184,10 +2184,10 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="3">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C140" s="2">
         <v>1</v>
@@ -2195,32 +2195,32 @@
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="3">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C141" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="3">
-        <v>45972</v>
+        <v>45974</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C142" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="3">
-        <v>45972</v>
+        <v>45974</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C143" s="2">
         <v>1</v>
@@ -2228,10 +2228,10 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="3">
-        <v>45972</v>
+        <v>45974</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C144" s="2">
         <v>1</v>
@@ -2239,32 +2239,32 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="3">
-        <v>45972</v>
+        <v>45974</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C145" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="3">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C146" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="3">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C147" s="2">
         <v>1</v>
@@ -2272,10 +2272,10 @@
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="3">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C148" s="2">
         <v>1</v>
@@ -2283,10 +2283,10 @@
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="3">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C149" s="2">
         <v>1</v>
@@ -2294,10 +2294,10 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="3">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C150" s="2">
         <v>1</v>
@@ -2308,10 +2308,10 @@
         <v>45974</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C151" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2319,10 +2319,10 @@
         <v>45974</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C152" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2330,7 +2330,7 @@
         <v>45974</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C153" s="2">
         <v>1</v>
@@ -2341,7 +2341,7 @@
         <v>45974</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C154" s="2">
         <v>1</v>
@@ -2352,7 +2352,7 @@
         <v>45974</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C155" s="2">
         <v>1</v>
@@ -2360,32 +2360,32 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="3">
-        <v>45975</v>
+        <v>45974</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C156" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="3">
-        <v>45975</v>
+        <v>45974</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C157" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="3">
-        <v>45975</v>
+        <v>45974</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C158" s="2">
         <v>1</v>
@@ -2393,10 +2393,10 @@
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="3">
-        <v>45975</v>
+        <v>45974</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C159" s="2">
         <v>1</v>
@@ -2404,10 +2404,10 @@
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="3">
-        <v>45975</v>
+        <v>45974</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C160" s="2">
         <v>1</v>
@@ -2415,32 +2415,32 @@
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="3">
-        <v>45976</v>
+        <v>45974</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C161" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="3">
-        <v>45976</v>
+        <v>45975</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C162" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="3">
-        <v>45976</v>
+        <v>45975</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C163" s="2">
         <v>1</v>
@@ -2448,10 +2448,10 @@
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="3">
-        <v>45976</v>
+        <v>45975</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C164" s="2">
         <v>1</v>
@@ -2459,32 +2459,32 @@
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="3">
-        <v>45976</v>
+        <v>45975</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C165" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="3">
-        <v>45977</v>
+        <v>45975</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C166" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="3">
-        <v>45977</v>
+        <v>45975</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C167" s="2">
         <v>1</v>
@@ -2492,10 +2492,10 @@
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="3">
-        <v>45977</v>
+        <v>45975</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C168" s="2">
         <v>1</v>
@@ -2503,10 +2503,10 @@
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="3">
-        <v>45977</v>
+        <v>45975</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C169" s="2">
         <v>1</v>
@@ -2514,10 +2514,10 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="3">
-        <v>45977</v>
+        <v>45975</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C170" s="2">
         <v>1</v>
@@ -2525,10 +2525,10 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="3">
-        <v>45964</v>
+        <v>45975</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C171" s="2">
         <v>1</v>
@@ -2536,21 +2536,21 @@
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="3">
-        <v>45964</v>
+        <v>45975</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C172" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="3">
-        <v>45965</v>
+        <v>45975</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C173" s="2">
         <v>1</v>
@@ -2558,10 +2558,10 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="3">
-        <v>45965</v>
+        <v>45975</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C174" s="2">
         <v>1</v>
@@ -2569,10 +2569,10 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="3">
-        <v>45966</v>
+        <v>45975</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C175" s="2">
         <v>1</v>
@@ -2580,10 +2580,10 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="3">
-        <v>45966</v>
+        <v>45975</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C176" s="2">
         <v>1</v>
@@ -2591,21 +2591,21 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="3">
-        <v>45967</v>
+        <v>45975</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="C177" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="3">
-        <v>45967</v>
+        <v>45975</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C178" s="2">
         <v>1</v>
@@ -2613,10 +2613,10 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="3">
-        <v>45968</v>
+        <v>45975</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C179" s="2">
         <v>1</v>
@@ -2624,10 +2624,10 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="3">
-        <v>45968</v>
+        <v>45975</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C180" s="2">
         <v>1</v>
@@ -2635,10 +2635,10 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="3">
-        <v>45969</v>
+        <v>45975</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C181" s="2">
         <v>1</v>
@@ -2646,21 +2646,21 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="3">
-        <v>45969</v>
+        <v>45976</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C182" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="3">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C183" s="2">
         <v>1</v>
@@ -2668,10 +2668,10 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="3">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C184" s="2">
         <v>1</v>
@@ -2679,32 +2679,32 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="3">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="C185" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="3">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C186" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="3">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C187" s="2">
         <v>1</v>
@@ -2712,10 +2712,10 @@
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="3">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C188" s="2">
         <v>1</v>
@@ -2723,10 +2723,10 @@
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="3">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C189" s="2">
         <v>1</v>
@@ -2734,10 +2734,10 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="3">
-        <v>45972</v>
+        <v>45976</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C190" s="2">
         <v>1</v>
@@ -2745,21 +2745,21 @@
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="3">
-        <v>45972</v>
+        <v>45976</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C191" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="3">
-        <v>45972</v>
+        <v>45976</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C192" s="2">
         <v>1</v>
@@ -2767,10 +2767,10 @@
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="3">
-        <v>45972</v>
+        <v>45976</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C193" s="2">
         <v>1</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="3">
-        <v>45972</v>
+        <v>45976</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C194" s="2">
         <v>1</v>
@@ -2789,10 +2789,10 @@
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="3">
-        <v>45973</v>
+        <v>45976</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C195" s="2">
         <v>1</v>
@@ -2800,32 +2800,32 @@
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="3">
-        <v>45973</v>
+        <v>45976</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="C196" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="3">
-        <v>45973</v>
+        <v>45976</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C197" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="3">
-        <v>45973</v>
+        <v>45976</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C198" s="2">
         <v>1</v>
@@ -2833,10 +2833,10 @@
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="3">
-        <v>45973</v>
+        <v>45976</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C199" s="2">
         <v>1</v>
@@ -2844,21 +2844,21 @@
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="3">
-        <v>45974</v>
+        <v>45976</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C200" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" s="3">
-        <v>45974</v>
+        <v>45976</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C201" s="2">
         <v>1</v>
@@ -2866,21 +2866,21 @@
     </row>
     <row r="202" spans="1:3">
       <c r="A202" s="3">
-        <v>45974</v>
+        <v>45977</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C202" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="3">
-        <v>45974</v>
+        <v>45977</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C203" s="2">
         <v>1</v>
@@ -2888,10 +2888,10 @@
     </row>
     <row r="204" spans="1:3">
       <c r="A204" s="3">
-        <v>45974</v>
+        <v>45977</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C204" s="2">
         <v>1</v>
@@ -2899,32 +2899,32 @@
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="3">
-        <v>45975</v>
+        <v>45977</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C205" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="3">
-        <v>45975</v>
+        <v>45977</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C206" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="3">
-        <v>45975</v>
+        <v>45977</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C207" s="2">
         <v>1</v>
@@ -2932,10 +2932,10 @@
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="3">
-        <v>45975</v>
+        <v>45977</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C208" s="2">
         <v>1</v>
@@ -2943,10 +2943,10 @@
     </row>
     <row r="209" spans="1:3">
       <c r="A209" s="3">
-        <v>45975</v>
+        <v>45977</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C209" s="2">
         <v>1</v>
@@ -2954,32 +2954,32 @@
     </row>
     <row r="210" spans="1:3">
       <c r="A210" s="3">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C210" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="3">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C211" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="3">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C212" s="2">
         <v>1</v>
@@ -2987,10 +2987,10 @@
     </row>
     <row r="213" spans="1:3">
       <c r="A213" s="3">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C213" s="2">
         <v>1</v>
@@ -2998,10 +2998,10 @@
     </row>
     <row r="214" spans="1:3">
       <c r="A214" s="3">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C214" s="2">
         <v>1</v>
@@ -3009,10 +3009,10 @@
     </row>
     <row r="215" spans="1:3">
       <c r="A215" s="3">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C215" s="2">
         <v>1</v>
@@ -3074,7 +3074,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C220" xr:uid="{23CD45F7-3C4B-E946-8B39-383CEB4DE523}"/>
+  <autoFilter ref="A1:C220" xr:uid="{23CD45F7-3C4B-E946-8B39-383CEB4DE523}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C220">
+      <sortCondition ref="A1:A220"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>